<commit_message>
Update Excel file with new data
</commit_message>
<xml_diff>
--- a/python/名簿・領収書.xlsx
+++ b/python/名簿・領収書.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\matu\work\ToDo\support-ac\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90839907-FDDA-4294-A66E-FEC04F16E528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A259773-CA37-43BD-95BD-82E828A728ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28905" yWindow="-3705" windowWidth="29010" windowHeight="32505" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="参加費" sheetId="1" r:id="rId1"/>
@@ -242,7 +242,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="#,##0_);[Red]\(#,##0\)"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -677,10 +677,10 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.77734375" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.44140625" style="1" customWidth="1"/>
@@ -692,7 +692,7 @@
     <col min="1019" max="1020" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -715,7 +715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -739,7 +739,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -763,7 +763,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -787,7 +787,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -811,7 +811,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -835,7 +835,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -859,7 +859,7 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -883,7 +883,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -907,7 +907,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
@@ -931,7 +931,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -955,7 +955,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
@@ -979,7 +979,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>29</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>31</v>
       </c>
@@ -1099,7 +1099,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>33</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>35</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>37</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>39</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>41</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>44</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>46</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>13000</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>48</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>50</v>
       </c>

</xml_diff>